<commit_message>
trigger settings for tek
</commit_message>
<xml_diff>
--- a/testsheets/666_Tektronix_TDS3034C.xlsx
+++ b/testsheets/666_Tektronix_TDS3034C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Python\oscilloscope\testsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A1EDAC2-42B5-4B9E-B8C0-226F7599BFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{FA4CDB5D-3F2C-4FD8-9A40-03D586C26547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="88">
   <si>
     <t>EMU Filename:</t>
   </si>
@@ -278,9 +278,6 @@
   </si>
   <si>
     <t>TRIG</t>
-  </si>
-  <si>
-    <t>AC</t>
   </si>
   <si>
     <t>Edge</t>
@@ -1193,8 +1190,8 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B68" workbookViewId="0">
+      <selection activeCell="N80" sqref="N80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1213,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3147,7 +3144,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>78</v>
@@ -3178,25 +3175,19 @@
         <v>51</v>
       </c>
       <c r="P79" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q79" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R79" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="S79" s="9" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="T79" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="U79" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="V79" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
@@ -3204,10 +3195,10 @@
         <v>41</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5" t="str">
@@ -3220,34 +3211,31 @@
       <c r="O80" s="9">
         <v>1</v>
       </c>
-      <c r="P80" s="9" t="s">
-        <v>80</v>
+      <c r="P80" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q80" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R80" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T80" s="9">
         <v>50</v>
       </c>
-      <c r="U80" s="9">
+      <c r="S80" s="9">
         <v>300</v>
       </c>
-      <c r="V80" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B81" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="str">
@@ -3260,34 +3248,31 @@
       <c r="O81" s="9">
         <v>1</v>
       </c>
-      <c r="P81" s="9" t="s">
-        <v>80</v>
+      <c r="P81" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q81" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R81" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T81" s="9">
         <v>50</v>
       </c>
-      <c r="U81" s="9">
+      <c r="S81" s="9">
         <v>300</v>
       </c>
-      <c r="V81" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T81" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="5" t="str">
@@ -3300,34 +3285,31 @@
       <c r="O82" s="9">
         <v>2</v>
       </c>
-      <c r="P82" s="9" t="s">
-        <v>80</v>
+      <c r="P82" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q82" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R82" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T82" s="9">
         <v>50</v>
       </c>
-      <c r="U82" s="9">
+      <c r="S82" s="9">
         <v>300</v>
       </c>
-      <c r="V82" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B83" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C83" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="str">
@@ -3340,34 +3322,31 @@
       <c r="O83" s="9">
         <v>2</v>
       </c>
-      <c r="P83" s="9" t="s">
-        <v>80</v>
+      <c r="P83" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q83" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R83" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T83" s="9">
         <v>50</v>
       </c>
-      <c r="U83" s="9">
+      <c r="S83" s="9">
         <v>300</v>
       </c>
-      <c r="V83" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="5" t="str">
@@ -3380,34 +3359,31 @@
       <c r="O84" s="9">
         <v>3</v>
       </c>
-      <c r="P84" s="9" t="s">
-        <v>80</v>
+      <c r="P84" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q84" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R84" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T84" s="9">
         <v>50</v>
       </c>
-      <c r="U84" s="9">
+      <c r="S84" s="9">
         <v>300</v>
       </c>
-      <c r="V84" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B85" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C85" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="str">
@@ -3420,34 +3396,31 @@
       <c r="O85" s="9">
         <v>3</v>
       </c>
-      <c r="P85" s="9" t="s">
-        <v>80</v>
+      <c r="P85" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q85" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R85" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T85" s="9">
         <v>50</v>
       </c>
-      <c r="U85" s="9">
+      <c r="S85" s="9">
         <v>300</v>
       </c>
-      <c r="V85" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T85" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
         <v>45</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="str">
@@ -3460,34 +3433,31 @@
       <c r="O86" s="9">
         <v>4</v>
       </c>
-      <c r="P86" s="9" t="s">
-        <v>80</v>
+      <c r="P86" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q86" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R86" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T86" s="9">
         <v>50</v>
       </c>
-      <c r="U86" s="9">
+      <c r="S86" s="9">
         <v>300</v>
       </c>
-      <c r="V86" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T86" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
         <v>45</v>
       </c>
       <c r="B87" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C87" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D87" s="19"/>
       <c r="E87" s="5" t="str">
@@ -3500,34 +3470,31 @@
       <c r="O87" s="9">
         <v>4</v>
       </c>
-      <c r="P87" s="9" t="s">
-        <v>80</v>
+      <c r="P87" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q87" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R87" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T87" s="9">
         <v>50</v>
       </c>
-      <c r="U87" s="9">
+      <c r="S87" s="9">
         <v>300</v>
       </c>
-      <c r="V87" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T87" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="str">
@@ -3540,34 +3507,31 @@
       <c r="O88" s="9">
         <v>1</v>
       </c>
-      <c r="P88" s="9" t="s">
-        <v>80</v>
+      <c r="P88" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q88" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R88" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T88" s="9">
         <v>50</v>
       </c>
-      <c r="U88" s="9">
+      <c r="S88" s="9">
         <v>50</v>
       </c>
-      <c r="V88" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B89" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5" t="str">
@@ -3580,34 +3544,31 @@
       <c r="O89" s="9">
         <v>1</v>
       </c>
-      <c r="P89" s="9" t="s">
-        <v>80</v>
+      <c r="P89" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q89" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R89" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T89" s="9">
         <v>50</v>
       </c>
-      <c r="U89" s="9">
+      <c r="S89" s="9">
         <v>50</v>
       </c>
-      <c r="V89" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T89" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="5" t="str">
@@ -3620,34 +3581,31 @@
       <c r="O90" s="9">
         <v>2</v>
       </c>
-      <c r="P90" s="9" t="s">
-        <v>80</v>
+      <c r="P90" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q90" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R90" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T90" s="9">
         <v>50</v>
       </c>
-      <c r="U90" s="9">
+      <c r="S90" s="9">
         <v>50</v>
       </c>
-      <c r="V90" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T90" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B91" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5" t="str">
@@ -3660,34 +3618,31 @@
       <c r="O91" s="9">
         <v>2</v>
       </c>
-      <c r="P91" s="9" t="s">
-        <v>80</v>
+      <c r="P91" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q91" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R91" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T91" s="9">
         <v>50</v>
       </c>
-      <c r="U91" s="9">
+      <c r="S91" s="9">
         <v>50</v>
       </c>
-      <c r="V91" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T91" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5" t="str">
@@ -3700,34 +3655,31 @@
       <c r="O92" s="9">
         <v>3</v>
       </c>
-      <c r="P92" s="9" t="s">
-        <v>80</v>
+      <c r="P92" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q92" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R92" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T92" s="9">
         <v>50</v>
       </c>
-      <c r="U92" s="9">
+      <c r="S92" s="9">
         <v>50</v>
       </c>
-      <c r="V92" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T92" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5" t="str">
@@ -3740,34 +3692,31 @@
       <c r="O93" s="9">
         <v>3</v>
       </c>
-      <c r="P93" s="9" t="s">
-        <v>80</v>
+      <c r="P93" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q93" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R93" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T93" s="9">
         <v>50</v>
       </c>
-      <c r="U93" s="9">
+      <c r="S93" s="9">
         <v>50</v>
       </c>
-      <c r="V93" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T93" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>45</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="5" t="str">
@@ -3780,34 +3729,31 @@
       <c r="O94" s="9">
         <v>4</v>
       </c>
-      <c r="P94" s="9" t="s">
-        <v>80</v>
+      <c r="P94" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q94" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R94" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T94" s="9">
         <v>50</v>
       </c>
-      <c r="U94" s="9">
+      <c r="S94" s="9">
         <v>50</v>
       </c>
-      <c r="V94" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T94" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>45</v>
       </c>
       <c r="B95" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D95" s="19"/>
       <c r="E95" s="5" t="str">
@@ -3820,23 +3766,20 @@
       <c r="O95" s="9">
         <v>4</v>
       </c>
-      <c r="P95" s="9" t="s">
-        <v>80</v>
+      <c r="P95" s="9">
+        <v>0.1</v>
       </c>
       <c r="Q95" s="9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="R95" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="T95" s="9">
         <v>50</v>
       </c>
-      <c r="U95" s="9">
+      <c r="S95" s="9">
         <v>50</v>
       </c>
-      <c r="V95" t="s">
-        <v>83</v>
+      <c r="T95" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update template to use invert settings
</commit_message>
<xml_diff>
--- a/testsheets/666_Tektronix_TDS3034C.xlsx
+++ b/testsheets/666_Tektronix_TDS3034C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Python\oscilloscope\testsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{FA4CDB5D-3F2C-4FD8-9A40-03D586C26547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2A154C3-5B44-4A39-8078-A0327EC59C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="89">
   <si>
     <t>EMU Filename:</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>PERFORMANCE TEST CARD (AS RECEIVED AND AS COMPLETED)</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -1190,8 +1193,8 @@
   </sheetPr>
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B68" workbookViewId="0">
-      <selection activeCell="N80" sqref="N80"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,6 +1751,9 @@
       <c r="T28" s="9">
         <v>150</v>
       </c>
+      <c r="V28" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -1821,7 +1827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>66</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
@@ -1907,7 +1913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>67</v>
       </c>
@@ -1947,7 +1953,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>67</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>72</v>
       </c>
@@ -2010,7 +2016,7 @@
         <v>Not Done</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>68</v>
       </c>
@@ -2050,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>33</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>70</v>
       </c>
@@ -2135,14 +2141,17 @@
       <c r="T40" s="9">
         <v>150</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>22</v>
       </c>
@@ -2165,7 +2174,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>63</v>
       </c>
@@ -2208,7 +2217,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>66</v>
       </c>
@@ -2251,7 +2260,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>32</v>
       </c>
@@ -2294,7 +2303,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>67</v>
       </c>
@@ -2334,7 +2343,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>67</v>
       </c>
@@ -2374,7 +2383,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -2397,7 +2406,7 @@
         <v>Not Done</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>68</v>
       </c>
@@ -2437,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>33</v>
       </c>
@@ -2480,7 +2489,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>70</v>
       </c>
@@ -2522,14 +2531,17 @@
       <c r="T52" s="9">
         <v>150</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>22</v>
       </c>
@@ -2552,7 +2564,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>63</v>
       </c>
@@ -2595,7 +2607,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>66</v>
       </c>
@@ -2638,7 +2650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>32</v>
       </c>
@@ -2681,7 +2693,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>67</v>
       </c>
@@ -2721,7 +2733,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>67</v>
       </c>
@@ -2761,7 +2773,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>72</v>
       </c>
@@ -2784,7 +2796,7 @@
         <v>Not Done</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>68</v>
       </c>
@@ -2824,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>33</v>
       </c>
@@ -2867,7 +2879,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>70</v>
       </c>
@@ -2908,6 +2920,9 @@
       </c>
       <c r="T64" s="9">
         <v>150</v>
+      </c>
+      <c r="V64" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3189,6 +3204,8 @@
       <c r="T79" s="9" t="s">
         <v>80</v>
       </c>
+      <c r="U79" s="9"/>
+      <c r="V79" s="9"/>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
@@ -3226,8 +3243,9 @@
       <c r="T80" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U80" s="9"/>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>41</v>
       </c>
@@ -3263,8 +3281,9 @@
       <c r="T81" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U81" s="9"/>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>43</v>
       </c>
@@ -3300,8 +3319,9 @@
       <c r="T82" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U82" s="9"/>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>43</v>
       </c>
@@ -3337,8 +3357,9 @@
       <c r="T83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U83" s="9"/>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>44</v>
       </c>
@@ -3374,8 +3395,9 @@
       <c r="T84" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U84" s="9"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>44</v>
       </c>
@@ -3411,8 +3433,9 @@
       <c r="T85" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U85" s="9"/>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
         <v>45</v>
       </c>
@@ -3448,8 +3471,9 @@
       <c r="T86" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U86" s="9"/>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
         <v>45</v>
       </c>
@@ -3485,8 +3509,9 @@
       <c r="T87" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U87" s="9"/>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>41</v>
       </c>
@@ -3522,8 +3547,9 @@
       <c r="T88" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U88" s="9"/>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>41</v>
       </c>
@@ -3559,8 +3585,9 @@
       <c r="T89" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U89" s="9"/>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
         <v>43</v>
       </c>
@@ -3596,8 +3623,9 @@
       <c r="T90" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U90" s="9"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
         <v>43</v>
       </c>
@@ -3633,8 +3661,9 @@
       <c r="T91" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U91" s="9"/>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>44</v>
       </c>
@@ -3670,8 +3699,9 @@
       <c r="T92" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U92" s="9"/>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>44</v>
       </c>
@@ -3707,8 +3737,9 @@
       <c r="T93" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U93" s="9"/>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>45</v>
       </c>
@@ -3744,8 +3775,9 @@
       <c r="T94" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U94" s="9"/>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>45</v>
       </c>
@@ -3781,6 +3813,7 @@
       <c r="T95" t="s">
         <v>82</v>
       </c>
+      <c r="U95" s="9"/>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="8" t="s">

</xml_diff>